<commit_message>
big model refactor, project dict works
</commit_message>
<xml_diff>
--- a/docs/wordcontrol_import_nirvi_example.xlsx
+++ b/docs/wordcontrol_import_nirvi_example.xlsx
@@ -19,12 +19,6 @@
     <t>Параметры лексем</t>
   </si>
   <si>
-    <t>Ижорский (сойкинский) [Nirvi @ Nirvi]</t>
-  </si>
-  <si>
-    <t>Ижорский (сойкинский) [учебная @ Nirvi в учебной]</t>
-  </si>
-  <si>
     <t>Финский</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>Расширенный комментарий</t>
+  </si>
+  <si>
+    <t>Ижорский (сойкинский) [Nirvi] @ Nirvi</t>
+  </si>
+  <si>
+    <t>Ижорский (сойкинский) [учебная] @ Nirvi | в учебной системе</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,118 +552,118 @@
     <col min="6" max="6" width="24" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yet another refactoring started
</commit_message>
<xml_diff>
--- a/docs/wordcontrol_import_nirvi_example.xlsx
+++ b/docs/wordcontrol_import_nirvi_example.xlsx
@@ -137,10 +137,10 @@
     <t>Расширенный комментарий</t>
   </si>
   <si>
-    <t>Ижорский (сойкинский) [Nirvi] @ Nirvi</t>
-  </si>
-  <si>
-    <t>Ижорский (сойкинский) [учебная] @ Nirvi | в учебной системе</t>
+    <t>Ижорский (сойкинский) [учебная] | в учебной системе</t>
+  </si>
+  <si>
+    <t>Ижорский (сойкинский) [Nirvi]</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,15 +552,15 @@
     <col min="6" max="6" width="24" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>

</xml_diff>